<commit_message>
Finished code for entering student information into student access, now working on adding functionality that will match the user data with the excel file.
</commit_message>
<xml_diff>
--- a/Sample Bnumber List.xlsx
+++ b/Sample Bnumber List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reyno\PycharmProjects\Student Access Data Entry Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209EB9E2-69EB-433C-A0B2-5FE65370F7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2312B38-5177-4E3D-9126-0198D152804D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{952E855C-B277-45F2-B072-F147F81CCE7D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>First Name</t>
   </si>
@@ -47,28 +47,25 @@
     <t>B Number</t>
   </si>
   <si>
-    <t>Reynoso-Perez</t>
-  </si>
-  <si>
-    <t>B00735305</t>
-  </si>
-  <si>
-    <t>Nyx</t>
-  </si>
-  <si>
-    <t>Elizebeth</t>
-  </si>
-  <si>
-    <t>Nichols</t>
-  </si>
-  <si>
-    <t>B00801848</t>
-  </si>
-  <si>
     <t>Middle Name</t>
   </si>
   <si>
-    <t>David</t>
+    <t>Test_one</t>
+  </si>
+  <si>
+    <t>Test_two</t>
+  </si>
+  <si>
+    <t>middle test</t>
+  </si>
+  <si>
+    <t>Middle test two</t>
+  </si>
+  <si>
+    <t>Last Name Test</t>
+  </si>
+  <si>
+    <t>Last Name Test 2</t>
   </si>
 </sst>
 </file>
@@ -423,14 +420,14 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="8.9296875" customWidth="1"/>
-    <col min="2" max="2" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
@@ -438,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -449,13 +446,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -463,13 +463,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed code to where it enters in student data. Next step is to make it so it opens a folder rather than having to input each file manually
</commit_message>
<xml_diff>
--- a/Sample Bnumber List.xlsx
+++ b/Sample Bnumber List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reyno\PycharmProjects\Student Access Data Entry Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2312B38-5177-4E3D-9126-0198D152804D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6815FBCF-8C28-4069-A74F-B8C6C864420C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{952E855C-B277-45F2-B072-F147F81CCE7D}"/>
+    <workbookView xWindow="2107" yWindow="2033" windowWidth="16201" windowHeight="9712" xr2:uid="{952E855C-B277-45F2-B072-F147F81CCE7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>First Name</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>Last Name Test 2</t>
+  </si>
+  <si>
+    <t>Test_three</t>
+  </si>
+  <si>
+    <t>Last Name Test 3</t>
+  </si>
+  <si>
+    <t>Middle three</t>
   </si>
 </sst>
 </file>
@@ -417,16 +426,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BAB3C68-1503-4411-AD5C-33A9BA42AF28}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.9296875" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -472,6 +481,20 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added feature that matches first name of both the excel and pdf, now to work on implementing it for last name in case there's multiple people with the same first name.
</commit_message>
<xml_diff>
--- a/Sample Bnumber List.xlsx
+++ b/Sample Bnumber List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reyno\PycharmProjects\Student Access Data Entry Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6815FBCF-8C28-4069-A74F-B8C6C864420C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81F90B3-4411-4AFD-BA1B-AB8C0234F760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2107" yWindow="2033" windowWidth="16201" windowHeight="9712" xr2:uid="{952E855C-B277-45F2-B072-F147F81CCE7D}"/>
+    <workbookView xWindow="3787" yWindow="1845" windowWidth="16200" windowHeight="9983" xr2:uid="{952E855C-B277-45F2-B072-F147F81CCE7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,45 +36,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>B Number</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
   <si>
     <t>First Name</t>
   </si>
   <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>B Number</t>
-  </si>
-  <si>
-    <t>Middle Name</t>
-  </si>
-  <si>
-    <t>Test_one</t>
-  </si>
-  <si>
-    <t>Test_two</t>
-  </si>
-  <si>
-    <t>middle test</t>
-  </si>
-  <si>
-    <t>Middle test two</t>
-  </si>
-  <si>
-    <t>Last Name Test</t>
-  </si>
-  <si>
-    <t>Last Name Test 2</t>
-  </si>
-  <si>
-    <t>Test_three</t>
-  </si>
-  <si>
-    <t>Last Name Test 3</t>
-  </si>
-  <si>
-    <t>Middle three</t>
+    <t xml:space="preserve">Jim </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jane </t>
+  </si>
+  <si>
+    <t>Aiden</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Maleficent</t>
+  </si>
+  <si>
+    <t>Jaundice</t>
   </si>
 </sst>
 </file>
@@ -429,28 +423,28 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -458,7 +452,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -472,10 +466,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -483,13 +477,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>3</v>

</xml_diff>